<commit_message>
fix: ajuste baseSap baseWms baseCiclico
</commit_message>
<xml_diff>
--- a/tmp/itens.xlsx
+++ b/tmp/itens.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\inventario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A6C2CD-CF1A-4845-829E-95BBBBA8D2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404E1863-8135-4C67-8613-6D71B641640D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2E7DCDE8-65B1-455A-9648-4E16BC7472AD}"/>
+    <workbookView xWindow="1545" yWindow="885" windowWidth="18345" windowHeight="10035" xr2:uid="{2E7DCDE8-65B1-455A-9648-4E16BC7472AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
   <dimension ref="A1:A37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix: ajuste baseCiclcio e create generateFichas
</commit_message>
<xml_diff>
--- a/tmp/itens.xlsx
+++ b/tmp/itens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\inventario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404E1863-8135-4C67-8613-6D71B641640D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F60349-0B6E-4D1A-9E18-D16E68F12A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1545" yWindow="885" windowWidth="18345" windowHeight="10035" xr2:uid="{2E7DCDE8-65B1-455A-9648-4E16BC7472AD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Item</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>0092-1290-0</t>
+  </si>
+  <si>
+    <t>0387-0199-01</t>
+  </si>
+  <si>
+    <t>0387-0199-03</t>
   </si>
 </sst>
 </file>
@@ -495,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565633A0-60F4-4C21-9E56-307D88C50101}">
-  <dimension ref="A1:A37"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,6 +697,21 @@
         <v>35</v>
       </c>
     </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>